<commit_message>
2022-11-21 NOJ: Combined components of conditions into a single cell, replaced operator labels with symbols, added quotation marks to comparison values, and tidied up.
</commit_message>
<xml_diff>
--- a/MC_plugin_configuration.xlsx
+++ b/MC_plugin_configuration.xlsx
@@ -43,7 +43,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -79,19 +79,13 @@
       <sz val="20"/>
     </font>
     <font>
-      <name val="Helvetica"/>
-      <family val="2"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-    </font>
-    <font>
       <name val="Tahoma"/>
       <family val="2"/>
       <color indexed="81"/>
       <sz val="8"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -104,14 +98,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF654EDA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -119,26 +107,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -152,14 +125,79 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1457,118 +1495,118 @@
     </row>
   </sheetData>
   <dataValidations count="38">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C18" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D18" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C19" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D19" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C20" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D20" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1583,7 +1621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1592,9 +1630,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="70.14999999999999" customWidth="1" min="1" max="1"/>
-    <col width="26.45" customWidth="1" min="2" max="2"/>
-    <col width="14.95" customWidth="1" min="3" max="3"/>
-    <col width="23" customWidth="1" min="4" max="4"/>
+    <col width="52.9" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1716,45 +1752,26 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>disposition_display</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>Call - No Answer</t>
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>“disposition_display” ≠ “Call - No Answer”</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="5" t="inlineStr">
+      <c r="A12" s="3" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C12" s="5" t="n"/>
-      <c r="D12" s="5" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>prospect</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>“prospect” ≠ “null”</t>
         </is>
       </c>
     </row>
@@ -2273,70 +2290,70 @@
     </row>
   </sheetData>
   <dataValidations count="22">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2351,7 +2368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2360,9 +2377,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="54.05" customWidth="1" min="1" max="1"/>
-    <col width="18.4" customWidth="1" min="2" max="2"/>
-    <col width="14.95" customWidth="1" min="3" max="3"/>
-    <col width="9.199999999999999" customWidth="1" min="4" max="4"/>
+    <col width="31.05" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2450,45 +2465,26 @@
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>delivered_at</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>“delivered_at” ≠ “null”</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="5" t="inlineStr">
+      <c r="A9" s="3" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C9" s="5" t="n"/>
-      <c r="D9" s="5" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>prospect</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>“prospect” ≠ “null”</t>
         </is>
       </c>
     </row>
@@ -3164,100 +3160,100 @@
     </row>
   </sheetData>
   <dataValidations count="32">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3272,7 +3268,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3281,9 +3277,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="70.14999999999999" customWidth="1" min="1" max="1"/>
-    <col width="14.95" customWidth="1" min="2" max="2"/>
-    <col width="14.95" customWidth="1" min="3" max="3"/>
-    <col width="10.35" customWidth="1" min="4" max="4"/>
+    <col width="27.6" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3405,97 +3399,58 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>action</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>call</t>
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>“action” ≠ “call”</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="5" t="inlineStr">
+      <c r="A12" s="3" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C12" s="5" t="n"/>
-      <c r="D12" s="5" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>action</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>email</t>
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>“action” ≠ “email”</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="5" t="inlineStr">
+      <c r="A14" s="3" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="5" t="inlineStr">
-        <is>
-          <t>action</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D15" s="5" t="inlineStr">
-        <is>
-          <t>sms</t>
+      <c r="A15" s="3" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>“action” ≠ “sms”</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="5" t="inlineStr">
+      <c r="A16" s="3" t="n"/>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C16" s="5" t="n"/>
-      <c r="D16" s="5" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>completed</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>equal</t>
-        </is>
-      </c>
-      <c r="D17" s="5" t="inlineStr">
-        <is>
-          <t>true</t>
+      <c r="A17" s="3" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>“completed” = “true”</t>
         </is>
       </c>
     </row>
@@ -4076,82 +4031,82 @@
     </row>
   </sheetData>
   <dataValidations count="26">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4166,7 +4121,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4175,9 +4130,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="70.14999999999999" customWidth="1" min="1" max="1"/>
-    <col width="19.55" customWidth="1" min="2" max="2"/>
-    <col width="14.95" customWidth="1" min="3" max="3"/>
-    <col width="10.35" customWidth="1" min="4" max="4"/>
+    <col width="27.6" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4275,71 +4228,42 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>prospect</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A9" s="3" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>“prospect” ≠ “null”</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="5" t="inlineStr">
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>canceled</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>equal</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>false</t>
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>“canceled” = “false”</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="5" t="inlineStr">
+      <c r="A12" s="3" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C12" s="5" t="n"/>
-      <c r="D12" s="5" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>organizer</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>equal</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>true</t>
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>“organizer” = “true”</t>
         </is>
       </c>
     </row>
@@ -4881,76 +4805,76 @@
     </row>
   </sheetData>
   <dataValidations count="24">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5471,16 +5395,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5837,10 +5761,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6176,16 +6100,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6602,34 +6526,34 @@
     </row>
   </sheetData>
   <dataValidations count="10">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7295,76 +7219,76 @@
     </row>
   </sheetData>
   <dataValidations count="24">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7976,64 +7900,64 @@
     </row>
   </sheetData>
   <dataValidations count="20">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8048,7 +7972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8058,8 +7982,6 @@
   <cols>
     <col width="80.5" customWidth="1" min="1" max="1"/>
     <col width="86.25" customWidth="1" min="2" max="2"/>
-    <col width="14.95" customWidth="1" min="3" max="3"/>
-    <col width="10.35" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8203,19 +8125,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>custom35</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>equal</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>“custom35” = “null”</t>
         </is>
       </c>
     </row>
@@ -8281,45 +8194,26 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="5" t="inlineStr">
-        <is>
-          <t>named_account</t>
-        </is>
-      </c>
-      <c r="C20" s="5" t="inlineStr">
-        <is>
-          <t>equal</t>
-        </is>
-      </c>
-      <c r="D20" s="5" t="inlineStr">
-        <is>
-          <t>false</t>
+      <c r="A20" s="3" t="n"/>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>“named_account” = “false”</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="5" t="inlineStr">
+      <c r="A21" s="3" t="n"/>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C21" s="5" t="n"/>
-      <c r="D21" s="5" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="5" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="C22" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D22" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A22" s="3" t="n"/>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>“owner” ≠ “null”</t>
         </is>
       </c>
     </row>
@@ -9978,214 +9872,214 @@
     </row>
   </sheetData>
   <dataValidations count="70">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C18" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D18" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C19" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D19" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C20" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D20" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C21" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D21" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C22" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D22" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C23" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D23" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C24" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D24" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C25" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D25" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C26" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D26" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C27" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D27" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C28" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D28" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C29" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D29" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C30" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D30" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C31" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D31" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C32" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D32" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C33" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D33" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C34" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D34" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C35" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D35" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C36" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D36" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C21" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D21" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C22" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D22" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C23" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D23" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C24" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D24" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C25" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D25" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C26" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D26" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C27" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D27" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C28" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D28" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C29" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D29" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C30" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D30" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C31" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D31" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C32" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D32" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C33" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D33" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C34" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D34" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C35" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D35" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C36" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D36" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10200,7 +10094,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10210,8 +10104,6 @@
   <cols>
     <col width="80.5" customWidth="1" min="1" max="1"/>
     <col width="86.25" customWidth="1" min="2" max="2"/>
-    <col width="14.95" customWidth="1" min="3" max="3"/>
-    <col width="25.3" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -10355,71 +10247,42 @@
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>custom33</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>012A0000000hjfGIAQ</t>
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>“custom33” ≠ “012A0000000hjfGIAQ”</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="5" t="inlineStr">
+      <c r="A14" s="3" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="5" t="inlineStr">
-        <is>
-          <t>custom33</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D15" s="5" t="inlineStr">
-        <is>
-          <t>012F00000013aTLIAY</t>
+      <c r="A15" s="3" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>“custom33” ≠ “012F00000013aTLIAY”</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="5" t="inlineStr">
+      <c r="A16" s="3" t="n"/>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
-      <c r="C16" s="5" t="n"/>
-      <c r="D16" s="5" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>custom33</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D17" s="5" t="inlineStr">
-        <is>
-          <t>0122A0000016MpTQAU</t>
+      <c r="A17" s="3" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>“custom33” ≠ “0122A0000016MpTQAU”</t>
         </is>
       </c>
     </row>
@@ -10485,45 +10348,26 @@
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="5" t="inlineStr">
-        <is>
-          <t>named_account</t>
-        </is>
-      </c>
-      <c r="C24" s="5" t="inlineStr">
-        <is>
-          <t>equal</t>
-        </is>
-      </c>
-      <c r="D24" s="5" t="inlineStr">
-        <is>
-          <t>true</t>
+      <c r="A24" s="3" t="n"/>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>“named_account” = “true”</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="5" t="inlineStr">
+      <c r="A25" s="3" t="n"/>
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C25" s="5" t="n"/>
-      <c r="D25" s="5" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="5" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="C26" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D26" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A26" s="3" t="n"/>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>“owner” ≠ “null”</t>
         </is>
       </c>
     </row>
@@ -11975,184 +11819,184 @@
     </row>
   </sheetData>
   <dataValidations count="60">
-    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C18" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D18" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C19" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D19" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C20" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D20" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C21" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D21" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C22" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D22" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C23" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D23" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C24" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D24" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C25" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D25" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C26" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D26" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C27" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D27" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C28" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D28" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C29" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D29" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C30" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D30" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C31" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D31" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D9" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D10" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D15" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C21" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D21" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C22" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D22" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C23" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D23" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C24" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D24" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C25" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D25" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C26" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D26" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C27" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D27" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C28" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D28" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C29" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D29" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C30" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D30" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C31" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Text,Number,Checkbox,Date/Time,Text (/Picklist),Lookup"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D31" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Record Data,Opt-Out,Outreach Engagement,Custom Fields"</formula1>
     </dataValidation>
   </dataValidations>
@@ -12167,7 +12011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12176,9 +12020,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="80.5" customWidth="1" min="1" max="1"/>
-    <col width="13.8" customWidth="1" min="2" max="2"/>
-    <col width="23" customWidth="1" min="3" max="3"/>
-    <col width="35.65" customWidth="1" min="4" max="4"/>
+    <col width="52.9" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12322,123 +12164,74 @@
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>does not contain</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>Mastercard</t>
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>“name” ⊅ “Mastercard”</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="5" t="inlineStr">
+      <c r="A14" s="3" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="5" t="inlineStr">
-        <is>
-          <t>domain</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>does not contain</t>
-        </is>
-      </c>
-      <c r="D15" s="5" t="inlineStr">
-        <is>
-          <t>mastercard.com</t>
+      <c r="A15" s="3" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>“domain” ⊅ “mastercard.com”</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="5" t="inlineStr">
+      <c r="A16" s="3" t="n"/>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>AND</t>
         </is>
       </c>
-      <c r="C16" s="5" t="n"/>
-      <c r="D16" s="5" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>custom35</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D17" s="5" t="inlineStr">
-        <is>
-          <t>MasterCard Employee</t>
+      <c r="A17" s="3" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>“custom35” ≠ “MasterCard Employee”</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="5" t="inlineStr">
+      <c r="A18" s="3" t="n"/>
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="5" t="inlineStr">
-        <is>
-          <t>custom35</t>
-        </is>
-      </c>
-      <c r="C19" s="5" t="inlineStr">
-        <is>
-          <t>does not contain</t>
-        </is>
-      </c>
-      <c r="D19" s="5" t="inlineStr">
-        <is>
-          <t>Start Path</t>
+      <c r="A19" s="3" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>“custom35” ⊅ “Start Path”</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="5" t="inlineStr">
+      <c r="A20" s="3" t="n"/>
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
-      <c r="C20" s="5" t="n"/>
-      <c r="D20" s="5" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="5" t="inlineStr">
-        <is>
-          <t>custom35</t>
-        </is>
-      </c>
-      <c r="C21" s="5" t="inlineStr">
-        <is>
-          <t>does not contain</t>
-        </is>
-      </c>
-      <c r="D21" s="5" t="inlineStr">
-        <is>
-          <t>NetZero/Sustainability Only</t>
+      <c r="A21" s="3" t="n"/>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>“custom35” ⊅ “NetZero/Sustainability Only”</t>
         </is>
       </c>
     </row>
@@ -12505,19 +12298,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="5" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="C29" s="5" t="inlineStr">
-        <is>
-          <t>not equal</t>
-        </is>
-      </c>
-      <c r="D29" s="5" t="inlineStr">
-        <is>
-          <t>null</t>
+      <c r="A29" s="3" t="n"/>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>“owner” ≠ “null”</t>
         </is>
       </c>
     </row>

</xml_diff>